<commit_message>
sections 1 & 2 modified
</commit_message>
<xml_diff>
--- a/01_Introducció/projectPlanning.xlsx
+++ b/01_Introducció/projectPlanning.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950"/>
@@ -16,26 +16,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Primer estudi superficial de l'API</t>
   </si>
   <si>
-    <t>Implementació de l'aplicació web</t>
-  </si>
-  <si>
     <t>Redacció de la memòria final</t>
   </si>
   <si>
     <t>Preparació de la presentació</t>
   </si>
   <si>
-    <t>9.5</t>
-  </si>
-  <si>
-    <t>10.5</t>
-  </si>
-  <si>
     <t>FASE DEL PROJECTE / SETMANA</t>
   </si>
   <si>
@@ -75,25 +66,22 @@
     <t>Generació d'idees per futurs projectes</t>
   </si>
   <si>
-    <t>6.5</t>
-  </si>
-  <si>
-    <t>7.5</t>
-  </si>
-  <si>
     <t>FASE DEL PROJECTE / MES</t>
   </si>
   <si>
     <t>Preparació de la defensa del projecte</t>
   </si>
   <si>
-    <t>Propostes de projecte per futurs estudiants i estudi de l'API</t>
-  </si>
-  <si>
     <t>Decisió i estudi de les tecnologies a utilitzar per l'aplicació web</t>
   </si>
   <si>
     <t>Decisió tipus d'aplicació a implementar i definició de l'estructura</t>
+  </si>
+  <si>
+    <t>Implementació de l'aplicació web i procés de certificació.</t>
+  </si>
+  <si>
+    <t>Estudi de l'API i elaboració de les propostes de projecte pels futurs estudiants.</t>
   </si>
 </sst>
 </file>
@@ -216,7 +204,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -286,6 +274,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -585,18 +576,18 @@
   <dimension ref="A1:AC14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+      <selection activeCell="X7" sqref="X7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="36.7109375" customWidth="1"/>
-    <col min="2" max="30" width="5.28515625" customWidth="1"/>
+    <col min="1" max="1" width="36.75" customWidth="1"/>
+    <col min="2" max="30" width="5.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="84.75" customHeight="1">
       <c r="A1" s="8" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B1" s="19">
         <v>42450</v>
@@ -687,12 +678,8 @@
       <c r="A2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4">
-        <v>1</v>
-      </c>
-      <c r="C2" s="4">
-        <v>2</v>
-      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
@@ -722,16 +709,12 @@
     </row>
     <row r="3" spans="1:29" ht="33" customHeight="1">
       <c r="A3" s="17" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
-      <c r="D3" s="4">
-        <v>1</v>
-      </c>
-      <c r="E3" s="4">
-        <v>2</v>
-      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
@@ -759,46 +742,26 @@
     </row>
     <row r="4" spans="1:29" ht="33" customHeight="1">
       <c r="A4" s="17" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
-      <c r="F4" s="4">
-        <v>1</v>
-      </c>
-      <c r="G4" s="4">
-        <v>2</v>
-      </c>
-      <c r="H4" s="4">
-        <v>3</v>
-      </c>
-      <c r="I4" s="4">
-        <v>4</v>
-      </c>
-      <c r="J4" s="4">
-        <v>5</v>
-      </c>
-      <c r="K4" s="4">
-        <v>6</v>
-      </c>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
       <c r="L4" s="6"/>
       <c r="M4" s="6"/>
       <c r="N4" s="6"/>
       <c r="O4" s="6"/>
-      <c r="P4" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q4" s="7">
-        <v>7</v>
-      </c>
-      <c r="R4" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="S4" s="7">
-        <v>8</v>
-      </c>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="7"/>
       <c r="T4" s="5"/>
       <c r="U4" s="5"/>
       <c r="V4" s="5"/>
@@ -812,56 +775,32 @@
     </row>
     <row r="5" spans="1:29" ht="33" customHeight="1">
       <c r="A5" s="17" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
-      <c r="F5" s="4">
-        <v>1</v>
-      </c>
-      <c r="G5" s="4">
-        <v>2</v>
-      </c>
-      <c r="H5" s="4">
-        <v>3</v>
-      </c>
-      <c r="I5" s="4">
-        <v>4</v>
-      </c>
-      <c r="J5" s="24">
-        <v>4.5</v>
-      </c>
-      <c r="K5" s="24">
-        <v>5</v>
-      </c>
-      <c r="L5" s="24">
-        <v>5.5</v>
-      </c>
-      <c r="M5" s="24">
-        <v>6</v>
-      </c>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="24"/>
+      <c r="K5" s="24"/>
+      <c r="L5" s="24"/>
+      <c r="M5" s="24"/>
+      <c r="N5" s="24"/>
+      <c r="O5" s="25"/>
       <c r="P5" s="5"/>
       <c r="Q5" s="5"/>
       <c r="R5" s="5"/>
       <c r="S5" s="5"/>
       <c r="T5" s="5"/>
       <c r="U5" s="21"/>
-      <c r="V5" s="24">
-        <v>6.5</v>
-      </c>
-      <c r="W5" s="24">
-        <v>7</v>
-      </c>
-      <c r="X5" s="24">
-        <v>7.5</v>
-      </c>
-      <c r="Y5" s="24">
-        <v>8</v>
-      </c>
+      <c r="V5" s="24"/>
+      <c r="W5" s="24"/>
+      <c r="X5" s="24"/>
+      <c r="Y5" s="24"/>
       <c r="Z5" s="21"/>
       <c r="AA5" s="5"/>
       <c r="AB5" s="5"/>
@@ -869,7 +808,7 @@
     </row>
     <row r="6" spans="1:29" ht="33" customHeight="1">
       <c r="A6" s="17" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -881,56 +820,28 @@
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
-      <c r="L6" s="4">
-        <v>1</v>
-      </c>
-      <c r="M6" s="4">
-        <v>2</v>
-      </c>
-      <c r="N6" s="4">
-        <v>3</v>
-      </c>
-      <c r="O6" s="4">
-        <v>4</v>
-      </c>
-      <c r="P6" s="4">
-        <v>5</v>
-      </c>
-      <c r="Q6" s="4">
-        <v>6</v>
-      </c>
-      <c r="R6" s="4">
-        <v>7</v>
-      </c>
-      <c r="S6" s="4">
-        <v>8</v>
-      </c>
-      <c r="T6" s="4">
-        <v>9</v>
-      </c>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
+      <c r="R6" s="4"/>
+      <c r="S6" s="4"/>
+      <c r="T6" s="4"/>
       <c r="U6" s="22"/>
-      <c r="V6" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="W6" s="7">
-        <v>10</v>
-      </c>
-      <c r="X6" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="Y6" s="7">
-        <v>11</v>
-      </c>
-      <c r="Z6" s="7">
-        <v>11.5</v>
-      </c>
+      <c r="V6" s="7"/>
+      <c r="W6" s="7"/>
+      <c r="X6" s="7"/>
+      <c r="Y6" s="7"/>
+      <c r="Z6" s="7"/>
       <c r="AA6" s="5"/>
       <c r="AB6" s="5"/>
       <c r="AC6" s="5"/>
     </row>
     <row r="7" spans="1:29" ht="33" customHeight="1">
       <c r="A7" s="18" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -951,33 +862,19 @@
       <c r="R7" s="5"/>
       <c r="S7" s="5"/>
       <c r="T7" s="5"/>
-      <c r="U7" s="4">
-        <v>1</v>
-      </c>
-      <c r="V7" s="4">
-        <v>2</v>
-      </c>
-      <c r="W7" s="4">
-        <v>3</v>
-      </c>
-      <c r="X7" s="4">
-        <v>4</v>
-      </c>
-      <c r="Y7" s="4">
-        <v>5</v>
-      </c>
-      <c r="Z7" s="4">
-        <v>6</v>
-      </c>
-      <c r="AA7" s="4">
-        <v>7</v>
-      </c>
+      <c r="U7" s="4"/>
+      <c r="V7" s="4"/>
+      <c r="W7" s="4"/>
+      <c r="X7" s="4"/>
+      <c r="Y7" s="4"/>
+      <c r="Z7" s="4"/>
+      <c r="AA7" s="4"/>
       <c r="AB7" s="5"/>
       <c r="AC7" s="5"/>
     </row>
     <row r="8" spans="1:29" ht="33" customHeight="1">
       <c r="A8" s="18" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -1005,12 +902,8 @@
       <c r="Y8" s="5"/>
       <c r="Z8" s="5"/>
       <c r="AA8" s="5"/>
-      <c r="AB8" s="4">
-        <v>1</v>
-      </c>
-      <c r="AC8" s="4">
-        <v>2</v>
-      </c>
+      <c r="AB8" s="4"/>
+      <c r="AC8" s="4"/>
     </row>
     <row r="9" spans="1:29" ht="29.25" customHeight="1"/>
     <row r="10" spans="1:29" ht="29.25" customHeight="1"/>
@@ -1021,9 +914,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="V6:Z6 P4:S4" numberStoredAsText="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -1037,39 +927,39 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" customWidth="1"/>
-    <col min="2" max="8" width="11.28515625" style="9" customWidth="1"/>
+    <col min="1" max="1" width="26.75" customWidth="1"/>
+    <col min="2" max="8" width="11.25" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="33" customHeight="1">
       <c r="A1" s="10" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C1" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="G1" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="H1" s="13" t="s">
         <v>9</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" s="13" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="33" customHeight="1">
       <c r="A2" s="23" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B2" s="15"/>
       <c r="C2" s="15"/>
@@ -1081,7 +971,7 @@
     </row>
     <row r="3" spans="1:8" ht="33" customHeight="1">
       <c r="A3" s="23" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="3"/>
@@ -1093,7 +983,7 @@
     </row>
     <row r="4" spans="1:8" ht="33" customHeight="1">
       <c r="A4" s="23" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="15"/>
@@ -1105,7 +995,7 @@
     </row>
     <row r="5" spans="1:8" ht="33" customHeight="1">
       <c r="A5" s="23" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -1117,7 +1007,7 @@
     </row>
     <row r="6" spans="1:8" ht="33" customHeight="1">
       <c r="A6" s="23" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -1129,7 +1019,7 @@
     </row>
     <row r="7" spans="1:8" ht="33" customHeight="1">
       <c r="A7" s="23" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>

</xml_diff>